<commit_message>
Epstein_l2 has been edited
</commit_message>
<xml_diff>
--- a/s2/epstein/Дроздов А.Д._Лаб-2_Вариант-4.xlsx
+++ b/s2/epstein/Дроздов А.Д._Лаб-2_Вариант-4.xlsx
@@ -12,16 +12,16 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Пример!$B$90:$C$90</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Пример!$B$101:$C$101</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Пример!$D$84</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Пример!$D$85</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Пример!$D$86</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Пример!$D$89</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Пример!$D$95</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Пример!$D$96</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Пример!$D$97</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Пример!$D$99</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">Пример!$E$96</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">Пример!$E$96</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">Пример!$E$96</definedName>
@@ -35,7 +35,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Пример!$D$82</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Пример!$D$93</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
@@ -46,10 +46,10 @@
     <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Пример!$E$84</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Пример!$E$85</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Пример!$E$86</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Пример!$E$89</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Пример!$E$95</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Пример!$E$96</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Пример!$E$97</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Пример!$E$99</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">Пример!$E$96</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">Пример!$E$96</definedName>
     <definedName name="solver_rhs7" localSheetId="0" hidden="1">Пример!$E$96</definedName>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
   <si>
     <t>A</t>
   </si>
@@ -381,31 +381,28 @@
     <t>maxh2</t>
   </si>
   <si>
-    <t>1.40</t>
-  </si>
-  <si>
-    <t>1.45</t>
-  </si>
-  <si>
-    <t>1.48</t>
-  </si>
-  <si>
-    <t>2.40</t>
-  </si>
-  <si>
-    <t>2.45</t>
-  </si>
-  <si>
-    <t>2.48</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> нет решения</t>
-  </si>
-  <si>
     <t>d3</t>
   </si>
   <si>
     <t>Max h2</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>1.55</t>
+  </si>
+  <si>
+    <t>1.60</t>
+  </si>
+  <si>
+    <t>2.50</t>
+  </si>
+  <si>
+    <t>2.55</t>
+  </si>
+  <si>
+    <t>2.60</t>
   </si>
 </sst>
 </file>
@@ -852,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -959,13 +956,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1289,14 +1280,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="15" max="15" width="24.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
+    <col min="17" max="18" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
@@ -1892,10 +1887,10 @@
       </c>
       <c r="I27" s="2">
         <f t="array" ref="I27:K27">TRANSPOSE(D31:D33)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J27" s="2">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="K27" s="2">
         <v>50</v>
@@ -1909,19 +1904,20 @@
         <v>1</v>
       </c>
       <c r="D28" s="14">
-        <f t="shared" ref="D28:D33" si="20">B28*B$34+C28*C$34</f>
+        <f t="shared" ref="D28:D30" si="20">B28*B$34+C28*C$34</f>
         <v>14</v>
       </c>
       <c r="E28" s="9">
+        <f>E3</f>
         <v>14</v>
       </c>
-      <c r="I28" s="28">
+      <c r="I28" s="26">
         <f>I27/I26</f>
-        <v>0.60869565217391308</v>
+        <v>0.82608695652173914</v>
       </c>
       <c r="J28" s="28">
         <f>J27/J26</f>
-        <v>0.48571428571428571</v>
+        <v>0.62857142857142856</v>
       </c>
       <c r="K28" s="26">
         <f>K27/K26</f>
@@ -1943,6 +1939,7 @@
         <v>34</v>
       </c>
       <c r="E29" s="9">
+        <f t="shared" ref="E29:E30" si="21">E4</f>
         <v>50</v>
       </c>
       <c r="I29" s="27"/>
@@ -1964,6 +1961,7 @@
         <v>50</v>
       </c>
       <c r="E30" s="9">
+        <f t="shared" si="21"/>
         <v>50</v>
       </c>
     </row>
@@ -1972,11 +1970,11 @@
         <v>1</v>
       </c>
       <c r="C31" s="8">
-        <v>1</v>
-      </c>
-      <c r="D31" s="49">
+        <v>2</v>
+      </c>
+      <c r="D31" s="46">
         <f>B31*B$34+C31*C$34</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G31" s="39"/>
     </row>
@@ -1985,11 +1983,11 @@
         <v>1</v>
       </c>
       <c r="C32" s="8">
-        <v>5</v>
-      </c>
-      <c r="D32" s="49">
+        <v>7</v>
+      </c>
+      <c r="D32" s="47">
         <f>B32*B$34+C32*C$34</f>
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E32" s="23"/>
     </row>
@@ -2000,7 +1998,7 @@
       <c r="C33" s="8">
         <v>1</v>
       </c>
-      <c r="D33" s="48">
+      <c r="D33" s="46">
         <f>B33*B$34+C33*C$34</f>
         <v>50</v>
       </c>
@@ -2020,8 +2018,8 @@
       </c>
     </row>
     <row r="36" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="43" t="s">
-        <v>34</v>
+      <c r="A36" s="41" t="s">
+        <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>20</v>
@@ -2046,18 +2044,18 @@
     </row>
     <row r="37" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C37" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37" s="2">
         <f>B37*B$45+C37*C$45</f>
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E37" s="14"/>
       <c r="G37" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H37" s="35">
         <v>40</v>
@@ -2087,13 +2085,16 @@
         <v>12</v>
       </c>
       <c r="H38" s="37">
-        <v>32</v>
+        <f>D37</f>
+        <v>23</v>
       </c>
       <c r="I38" s="37">
-        <v>29.6</v>
+        <f>D48</f>
+        <v>23</v>
       </c>
       <c r="J38" s="38">
-        <v>28.4</v>
+        <f>D59</f>
+        <v>23</v>
       </c>
       <c r="O38" s="14" t="s">
         <v>3</v>
@@ -2106,15 +2107,15 @@
       </c>
       <c r="R38" s="14">
         <f>I41/P38</f>
-        <v>0.92500000000000004</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="S38" s="14">
         <f>U38/U40</f>
-        <v>1</v>
+        <v>-10.399999999999928</v>
       </c>
       <c r="U38">
         <f>1-R38</f>
-        <v>7.4999999999999956E-2</v>
+        <v>0.54166666666666674</v>
       </c>
       <c r="V38">
         <v>2</v>
@@ -2131,23 +2132,27 @@
         <v>1</v>
       </c>
       <c r="D39" s="2">
-        <f t="shared" ref="D39:D44" si="21">B39*B$45+C39*C$45</f>
+        <f t="shared" ref="D39:D44" si="22">B39*B$45+C39*C$45</f>
         <v>14</v>
       </c>
       <c r="E39" s="2">
+        <f>E3</f>
         <v>14</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>4</v>
       </c>
       <c r="H39" s="21">
-        <v>41</v>
+        <f>D43</f>
+        <v>68.000000000000014</v>
       </c>
       <c r="I39" s="21">
-        <v>41</v>
+        <f>D54</f>
+        <v>68.000000000000014</v>
       </c>
       <c r="J39" s="22">
-        <v>41</v>
+        <f>D65</f>
+        <v>68</v>
       </c>
       <c r="O39" s="14" t="s">
         <v>4</v>
@@ -2157,18 +2162,18 @@
       </c>
       <c r="Q39" s="14">
         <f>I39/I40</f>
-        <v>1</v>
+        <v>1.5937500000000004</v>
       </c>
       <c r="R39" s="14">
         <v>1</v>
       </c>
       <c r="S39" s="14">
         <f>U39/U40</f>
-        <v>0</v>
+        <v>11.399999999999928</v>
       </c>
       <c r="U39">
         <f>1-Q39</f>
-        <v>0</v>
+        <v>-0.59375000000000044</v>
       </c>
       <c r="V39">
         <v>7</v>
@@ -2185,30 +2190,34 @@
         <v>5</v>
       </c>
       <c r="D40" s="2">
-        <f t="shared" si="21"/>
-        <v>34</v>
+        <f t="shared" si="22"/>
+        <v>50.000000000000007</v>
       </c>
       <c r="E40" s="2">
+        <f t="shared" ref="E40:E41" si="23">E4</f>
         <v>50</v>
       </c>
       <c r="G40" s="15" t="s">
         <v>33</v>
       </c>
       <c r="H40" s="16">
-        <v>41</v>
+        <f>D71</f>
+        <v>46</v>
       </c>
       <c r="I40" s="16">
-        <v>41</v>
+        <f>D82</f>
+        <v>42.666666666666664</v>
       </c>
       <c r="J40" s="17">
-        <v>35.6</v>
+        <f>D93</f>
+        <v>39.333333333333329</v>
       </c>
       <c r="O40" t="s">
         <v>18</v>
       </c>
       <c r="U40">
         <f>SUM(U38:U39)</f>
-        <v>7.4999999999999956E-2</v>
+        <v>-5.2083333333333703E-2</v>
       </c>
     </row>
     <row r="41" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2219,88 +2228,97 @@
         <v>1</v>
       </c>
       <c r="D41" s="2">
-        <f t="shared" si="21"/>
-        <v>50</v>
+        <f t="shared" si="22"/>
+        <v>33.999999999999993</v>
       </c>
       <c r="E41" s="2">
+        <f t="shared" si="23"/>
         <v>50</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>3</v>
       </c>
       <c r="H41" s="21">
-        <v>32</v>
+        <f>D76</f>
+        <v>20</v>
       </c>
       <c r="I41" s="21">
-        <v>29.6</v>
+        <f>D87</f>
+        <v>14.666666666666666</v>
       </c>
       <c r="J41" s="22">
-        <v>28.4</v>
+        <f>D98</f>
+        <v>21.666666666666664</v>
       </c>
       <c r="N41" s="1"/>
       <c r="O41" s="1">
         <f>SUMPRODUCT($S38:$S39,V38:V39)</f>
-        <v>2</v>
+        <v>58.999999999999645</v>
       </c>
       <c r="P41" s="1">
         <f>SUMPRODUCT($S38:$S39,W38:W39)</f>
-        <v>3</v>
+        <v>-19.799999999999855</v>
       </c>
     </row>
     <row r="42" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="5">
-        <v>3</v>
-      </c>
-      <c r="C42" s="5">
-        <v>1</v>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" si="21"/>
-        <v>32</v>
+        <f t="shared" si="22"/>
+        <v>23</v>
       </c>
       <c r="E42" s="5"/>
       <c r="G42" s="15" t="s">
         <v>10</v>
       </c>
       <c r="H42" s="16">
-        <v>9</v>
+        <f t="array" ref="H42:H43">TRANSPOSE(B79:C79)</f>
+        <v>8</v>
       </c>
       <c r="I42" s="16">
-        <v>7.7999999999980529</v>
+        <f t="array" ref="I42:I43">TRANSPOSE(B90:C90)</f>
+        <v>7.1666666666666661</v>
       </c>
       <c r="J42" s="17">
-        <v>7.1999999999955691</v>
+        <f t="array" ref="J42:J43">TRANSPOSE(B101:C101)</f>
+        <v>6.333333333333333</v>
       </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="V42">
         <f>S39*V39</f>
-        <v>0</v>
+        <v>79.7999999999995</v>
       </c>
     </row>
     <row r="43" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="40">
-        <v>4</v>
-      </c>
-      <c r="C43" s="41">
-        <v>1</v>
-      </c>
-      <c r="D43" s="41">
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>7</v>
+      </c>
+      <c r="D43" s="40">
         <f>B43*B$45+C43*C$45</f>
-        <v>41</v>
-      </c>
-      <c r="E43" s="42"/>
+        <v>68.000000000000014</v>
+      </c>
+      <c r="E43" s="3">
+        <v>50</v>
+      </c>
       <c r="G43" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H43" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I43" s="21">
-        <v>6.2000000000006423</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="J43" s="22">
-        <v>6.800000000003477</v>
+        <v>7.6666666666666661</v>
       </c>
       <c r="N43" s="1"/>
       <c r="O43" t="s">
@@ -2309,22 +2327,19 @@
       <c r="P43" s="1"/>
       <c r="V43">
         <f>S38*V38</f>
-        <v>2</v>
+        <v>-20.799999999999855</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B44" s="3">
-        <v>1</v>
-      </c>
-      <c r="C44" s="3">
-        <v>6</v>
+      <c r="B44" s="2">
+        <v>5</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
       </c>
       <c r="D44" s="3">
-        <f t="shared" si="21"/>
-        <v>39</v>
-      </c>
-      <c r="E44" s="3">
-        <v>40</v>
+        <f t="shared" si="22"/>
+        <v>33.999999999999993</v>
       </c>
       <c r="N44" s="1"/>
       <c r="O44" s="2">
@@ -2340,15 +2355,15 @@
       <c r="R44" s="14"/>
       <c r="V44">
         <f>SUM(V42:V43)</f>
-        <v>2</v>
+        <v>58.999999999999645</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
-        <v>9</v>
+        <v>4.9999999999999982</v>
       </c>
       <c r="C45" s="2">
-        <v>5</v>
+        <v>9.0000000000000018</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -2359,7 +2374,7 @@
         <v>1</v>
       </c>
       <c r="Q45" s="14">
-        <f t="shared" ref="Q45:Q50" si="22">SUMPRODUCT(O$51:P$51,O45:P45)</f>
+        <f t="shared" ref="Q45:Q50" si="24">SUMPRODUCT(O$51:P$51,O45:P45)</f>
         <v>14</v>
       </c>
       <c r="R45" s="2">
@@ -2377,7 +2392,7 @@
         <v>5</v>
       </c>
       <c r="Q46" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>38.799999999999997</v>
       </c>
       <c r="R46" s="2">
@@ -2385,14 +2400,14 @@
       </c>
     </row>
     <row r="47" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="43" t="s">
-        <v>35</v>
+      <c r="A47" s="41" t="s">
+        <v>37</v>
       </c>
       <c r="B47" t="s">
         <v>20</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I47" s="2">
         <v>40</v>
@@ -2410,7 +2425,7 @@
         <v>1</v>
       </c>
       <c r="Q47" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>45.2</v>
       </c>
       <c r="R47" s="2">
@@ -2419,14 +2434,14 @@
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C48" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48" s="2">
         <f>B48*B$56+C48*C$56</f>
-        <v>29.599999999999998</v>
+        <v>23</v>
       </c>
       <c r="E48" s="14"/>
       <c r="H48" s="15" t="s">
@@ -2448,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="Q48" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>29.599999999999998</v>
       </c>
       <c r="R48" s="14"/>
@@ -2477,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="Q49" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>37.4</v>
       </c>
       <c r="R49" s="26"/>
@@ -2494,6 +2509,7 @@
         <v>14</v>
       </c>
       <c r="E50" s="2">
+        <f>E3</f>
         <v>14</v>
       </c>
       <c r="O50" s="2">
@@ -2503,7 +2519,7 @@
         <v>6</v>
       </c>
       <c r="Q50" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>45</v>
       </c>
       <c r="R50" s="14">
@@ -2519,9 +2535,10 @@
       </c>
       <c r="D51" s="2">
         <f>B51*B$56+C51*C$56</f>
-        <v>38.799999999999997</v>
+        <v>50</v>
       </c>
       <c r="E51" s="2">
+        <f t="shared" ref="E51:E52" si="25">E4</f>
         <v>50</v>
       </c>
       <c r="O51" s="2">
@@ -2542,9 +2559,10 @@
       </c>
       <c r="D52" s="2">
         <f>B52*B$56+C52*C$56</f>
-        <v>45.2</v>
+        <v>34</v>
       </c>
       <c r="E52" s="2">
+        <f t="shared" si="25"/>
         <v>50</v>
       </c>
       <c r="H52" t="s">
@@ -2552,19 +2570,19 @@
       </c>
     </row>
     <row r="53" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="5">
-        <v>3</v>
-      </c>
-      <c r="C53" s="5">
-        <v>1</v>
+      <c r="B53" s="2">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2">
+        <v>2</v>
       </c>
       <c r="D53" s="5">
         <f>B53*B$56+C53*C$56</f>
-        <v>29.599999999999998</v>
+        <v>23</v>
       </c>
       <c r="E53" s="5"/>
       <c r="H53" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I53" s="2">
         <v>40</v>
@@ -2577,20 +2595,20 @@
       </c>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="40">
-        <v>4</v>
-      </c>
-      <c r="C54" s="41">
-        <v>1</v>
-      </c>
-      <c r="D54" s="41">
-        <f t="shared" ref="D54" si="23">B54*B$45+C54*C$45</f>
-        <v>41</v>
-      </c>
-      <c r="E54" s="42">
-        <v>0</v>
-      </c>
-      <c r="H54" s="44" t="s">
+      <c r="B54" s="2">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2">
+        <v>7</v>
+      </c>
+      <c r="D54" s="40">
+        <f>B54*B$45+C54*C$45</f>
+        <v>68.000000000000014</v>
+      </c>
+      <c r="E54" s="3">
+        <v>55</v>
+      </c>
+      <c r="H54" s="42" t="s">
         <v>12</v>
       </c>
       <c r="I54" s="37">
@@ -2607,29 +2625,26 @@
       </c>
     </row>
     <row r="55" spans="1:20" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="3">
-        <v>1</v>
-      </c>
-      <c r="C55" s="3">
-        <v>6</v>
+      <c r="B55" s="2">
+        <v>5</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1</v>
       </c>
       <c r="D55" s="3">
         <f>B55*B$56+C55*C$56</f>
-        <v>45</v>
-      </c>
-      <c r="E55" s="3">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I55" s="45">
+      <c r="I55" s="43">
         <v>41</v>
       </c>
       <c r="J55" s="2">
         <v>41</v>
       </c>
-      <c r="K55" s="45">
+      <c r="K55" s="43">
         <v>41</v>
       </c>
       <c r="O55" s="29">
@@ -2656,15 +2671,15 @@
     </row>
     <row r="56" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="2">
-        <v>7.8</v>
+        <v>5</v>
       </c>
       <c r="C56" s="2">
-        <v>6.2</v>
+        <v>9</v>
       </c>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
-      <c r="H56" s="46" t="s">
-        <v>42</v>
+      <c r="H56" s="44" t="s">
+        <v>35</v>
       </c>
       <c r="I56" s="16">
         <v>41</v>
@@ -2689,16 +2704,16 @@
         <v>92.5</v>
       </c>
       <c r="S56" s="21">
-        <f t="shared" ref="S56:T56" si="24">P55/P56*100</f>
+        <f t="shared" ref="S56:T56" si="26">P55/P56*100</f>
         <v>62.333333333333329</v>
       </c>
       <c r="T56" s="22">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>64.285714285714292</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H57" s="46" t="s">
+      <c r="H57" s="44" t="s">
         <v>29</v>
       </c>
       <c r="I57" s="2">
@@ -2712,13 +2727,13 @@
       </c>
     </row>
     <row r="58" spans="1:20" ht="18" x14ac:dyDescent="0.25">
-      <c r="A58" s="43" t="s">
-        <v>36</v>
+      <c r="A58" s="41" t="s">
+        <v>38</v>
       </c>
       <c r="B58" t="s">
         <v>20</v>
       </c>
-      <c r="H58" s="47" t="s">
+      <c r="H58" s="45" t="s">
         <v>30</v>
       </c>
       <c r="I58" s="16">
@@ -2733,17 +2748,17 @@
     </row>
     <row r="59" spans="1:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C59" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D59" s="2">
         <f>B59*B$67+C59*C$67</f>
-        <v>28.4</v>
+        <v>23</v>
       </c>
       <c r="E59" s="14"/>
-      <c r="H59" s="47" t="s">
+      <c r="H59" s="45" t="s">
         <v>31</v>
       </c>
       <c r="I59" s="21">
@@ -2788,10 +2803,11 @@
         <v>1</v>
       </c>
       <c r="D61" s="2">
-        <f t="shared" ref="D61:D66" si="25">B61*B$67+C61*C$67</f>
+        <f t="shared" ref="D61:D66" si="27">B61*B$67+C61*C$67</f>
         <v>14</v>
       </c>
       <c r="E61" s="2">
+        <f>E3</f>
         <v>14</v>
       </c>
       <c r="O61" s="20">
@@ -2821,10 +2837,11 @@
         <v>5</v>
       </c>
       <c r="D62" s="2">
-        <f t="shared" si="25"/>
-        <v>41.2</v>
+        <f t="shared" si="27"/>
+        <v>50</v>
       </c>
       <c r="E62" s="2">
+        <f t="shared" ref="E62:E63" si="28">E4</f>
         <v>50</v>
       </c>
     </row>
@@ -2836,67 +2853,67 @@
         <v>1</v>
       </c>
       <c r="D63" s="2">
-        <f t="shared" si="25"/>
-        <v>42.8</v>
+        <f t="shared" si="27"/>
+        <v>34</v>
       </c>
       <c r="E63" s="2">
+        <f t="shared" si="28"/>
         <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="5">
-        <v>3</v>
-      </c>
-      <c r="C64" s="5">
-        <v>1</v>
+      <c r="B64" s="2">
+        <v>1</v>
+      </c>
+      <c r="C64" s="2">
+        <v>2</v>
       </c>
       <c r="D64" s="5">
-        <f t="shared" si="25"/>
-        <v>28.4</v>
+        <f t="shared" si="27"/>
+        <v>23</v>
       </c>
       <c r="E64" s="5"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="40">
-        <v>4</v>
-      </c>
-      <c r="C65" s="41">
-        <v>1</v>
-      </c>
-      <c r="D65" s="41">
-        <f t="shared" si="25"/>
-        <v>35.599999999999994</v>
-      </c>
-      <c r="E65" s="42"/>
+      <c r="B65" s="2">
+        <v>1</v>
+      </c>
+      <c r="C65" s="2">
+        <v>7</v>
+      </c>
+      <c r="D65" s="40">
+        <f t="shared" si="27"/>
+        <v>68</v>
+      </c>
+      <c r="E65" s="3">
+        <v>60</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="3">
-        <v>1</v>
-      </c>
-      <c r="C66" s="3">
-        <v>6</v>
+      <c r="B66" s="2">
+        <v>5</v>
+      </c>
+      <c r="C66" s="2">
+        <v>1</v>
       </c>
       <c r="D66" s="3">
-        <f t="shared" si="25"/>
-        <v>48</v>
-      </c>
-      <c r="E66" s="3">
-        <v>48</v>
+        <f t="shared" si="27"/>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
-        <v>7.1999999999999993</v>
+        <v>4.9999999999999991</v>
       </c>
       <c r="C67" s="2">
-        <v>6.8000000000000007</v>
+        <v>9</v>
       </c>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="43" t="s">
-        <v>37</v>
+      <c r="A70" s="41" t="s">
+        <v>39</v>
       </c>
       <c r="B70" t="s">
         <v>20</v>
@@ -2904,14 +2921,14 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C71" s="2">
         <v>1</v>
       </c>
       <c r="D71" s="2">
         <f>B71*B$79+C71*C$79</f>
-        <v>40.400000000000006</v>
+        <v>46</v>
       </c>
       <c r="E71" s="14"/>
     </row>
@@ -2929,10 +2946,11 @@
         <v>1</v>
       </c>
       <c r="D73" s="2">
-        <f t="shared" ref="D73:D78" si="26">B73*B$79+C73*C$79</f>
+        <f t="shared" ref="D73:D78" si="29">B73*B$79+C73*C$79</f>
         <v>14</v>
       </c>
       <c r="E73" s="2">
+        <f>E3</f>
         <v>14</v>
       </c>
     </row>
@@ -2944,10 +2962,11 @@
         <v>5</v>
       </c>
       <c r="D74" s="2">
-        <f t="shared" si="26"/>
-        <v>34.799999999999997</v>
+        <f t="shared" si="29"/>
+        <v>38</v>
       </c>
       <c r="E74" s="2">
+        <f t="shared" ref="E74:E75" si="30">E4</f>
         <v>50</v>
       </c>
     </row>
@@ -2959,95 +2978,92 @@
         <v>1</v>
       </c>
       <c r="D75" s="2">
-        <f t="shared" si="26"/>
-        <v>49.2</v>
+        <f t="shared" si="29"/>
+        <v>46</v>
       </c>
       <c r="E75" s="2">
+        <f t="shared" si="30"/>
         <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="5">
-        <v>3</v>
-      </c>
-      <c r="C76" s="5">
-        <v>1</v>
+      <c r="B76" s="2">
+        <v>1</v>
+      </c>
+      <c r="C76" s="2">
+        <v>2</v>
       </c>
       <c r="D76" s="5">
-        <f t="shared" si="26"/>
-        <v>31.6</v>
+        <f t="shared" si="29"/>
+        <v>20</v>
       </c>
       <c r="E76" s="5"/>
     </row>
     <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="40">
-        <v>4</v>
-      </c>
-      <c r="C77" s="41">
-        <v>1</v>
-      </c>
-      <c r="D77" s="41">
-        <f t="shared" si="26"/>
-        <v>40.400000000000006</v>
-      </c>
-      <c r="E77" s="42"/>
+      <c r="B77" s="2">
+        <v>1</v>
+      </c>
+      <c r="C77" s="2">
+        <v>7</v>
+      </c>
+      <c r="D77" s="40">
+        <f t="shared" si="29"/>
+        <v>50</v>
+      </c>
+      <c r="E77" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="3">
-        <v>1</v>
-      </c>
-      <c r="C78" s="3">
-        <v>6</v>
+      <c r="B78" s="2">
+        <v>5</v>
+      </c>
+      <c r="C78" s="2">
+        <v>1</v>
       </c>
       <c r="D78" s="3">
-        <f t="shared" si="26"/>
-        <v>40</v>
-      </c>
-      <c r="E78" s="3">
-        <v>40</v>
+        <f t="shared" si="29"/>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" s="2">
-        <v>8.8000000000000007</v>
+        <v>8</v>
       </c>
       <c r="C79" s="2">
-        <v>5.1999999999999993</v>
+        <v>6</v>
       </c>
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="43" t="s">
-        <v>38</v>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="41" t="s">
+        <v>40</v>
       </c>
       <c r="B81" t="s">
         <v>20</v>
       </c>
-      <c r="F81" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B82" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C82" s="2">
         <v>1</v>
       </c>
       <c r="D82" s="2">
         <f>B82*B$90+C82*C$90</f>
-        <v>37.4</v>
+        <v>42.666666666666664</v>
       </c>
       <c r="E82" s="14"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
       <c r="E83" s="14"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B84" s="2">
         <v>1</v>
       </c>
@@ -3059,10 +3075,11 @@
         <v>14</v>
       </c>
       <c r="E84" s="2">
+        <f>E3</f>
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B85" s="2">
         <v>1</v>
       </c>
@@ -3071,13 +3088,14 @@
       </c>
       <c r="D85" s="2">
         <f>B85*B$90+C85*C$90</f>
-        <v>38.799999999999997</v>
+        <v>41.333333333333329</v>
       </c>
       <c r="E85" s="2">
+        <f t="shared" ref="E85:E86" si="31">E4</f>
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B86" s="2">
         <v>5</v>
       </c>
@@ -3086,93 +3104,93 @@
       </c>
       <c r="D86" s="2">
         <f>B86*B$90+C86*C$90</f>
-        <v>45.2</v>
+        <v>42.666666666666664</v>
       </c>
       <c r="E86" s="2">
+        <f t="shared" si="31"/>
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="5">
-        <v>3</v>
-      </c>
-      <c r="C87" s="5">
-        <v>1</v>
+    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="2">
+        <v>1</v>
+      </c>
+      <c r="C87" s="2">
+        <v>2</v>
       </c>
       <c r="D87" s="5">
         <f>B87*B$8+C87*C$90</f>
-        <v>9.1999999999999993</v>
+        <v>14.666666666666666</v>
       </c>
       <c r="E87" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="40">
-        <v>4</v>
-      </c>
-      <c r="C88" s="41">
-        <v>1</v>
-      </c>
-      <c r="D88" s="41">
+    <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="2">
+        <v>1</v>
+      </c>
+      <c r="C88" s="2">
+        <v>7</v>
+      </c>
+      <c r="D88" s="40">
         <f>B88*B$90+C88*C$90</f>
-        <v>37.4</v>
-      </c>
-      <c r="E88" s="42"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B89" s="3">
-        <v>1</v>
-      </c>
-      <c r="C89" s="3">
-        <v>6</v>
+        <v>54.999999999999993</v>
+      </c>
+      <c r="E88" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="2">
+        <v>5</v>
+      </c>
+      <c r="C89" s="2">
+        <v>1</v>
       </c>
       <c r="D89" s="3">
         <f>B89*B$90+C89*C$90</f>
-        <v>45</v>
-      </c>
-      <c r="E89" s="3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42.666666666666664</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B90" s="2">
-        <v>7.8</v>
+        <v>7.1666666666666661</v>
       </c>
       <c r="C90" s="2">
-        <v>6.2</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="43" t="s">
-        <v>39</v>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="41" t="s">
+        <v>41</v>
       </c>
       <c r="B92" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B93" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C93" s="2">
         <v>1</v>
       </c>
       <c r="D93" s="2">
         <f>B93*B$101+C93*C$101</f>
-        <v>35.599999999999994</v>
+        <v>39.333333333333329</v>
       </c>
       <c r="E93" s="14"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="14"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B95" s="2">
         <v>1</v>
       </c>
@@ -3180,14 +3198,15 @@
         <v>1</v>
       </c>
       <c r="D95" s="2">
-        <f t="shared" ref="D95:D100" si="27">B95*B$101+C95*C$101</f>
+        <f t="shared" ref="D95:D100" si="32">B95*B$101+C95*C$101</f>
         <v>14</v>
       </c>
       <c r="E95" s="2">
+        <f>E3</f>
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B96" s="2">
         <v>1</v>
       </c>
@@ -3195,10 +3214,11 @@
         <v>5</v>
       </c>
       <c r="D96" s="2">
-        <f t="shared" si="27"/>
-        <v>41.2</v>
+        <f t="shared" si="32"/>
+        <v>44.666666666666664</v>
       </c>
       <c r="E96" s="2">
+        <f t="shared" ref="E96:E97" si="33">E4</f>
         <v>50</v>
       </c>
     </row>
@@ -3210,62 +3230,60 @@
         <v>1</v>
       </c>
       <c r="D97" s="2">
-        <f t="shared" si="27"/>
-        <v>42.8</v>
+        <f t="shared" si="32"/>
+        <v>39.333333333333329</v>
       </c>
       <c r="E97" s="2">
+        <f t="shared" si="33"/>
         <v>50</v>
       </c>
     </row>
     <row r="98" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="5">
-        <v>3</v>
-      </c>
-      <c r="C98" s="5">
-        <v>1</v>
+      <c r="B98" s="2">
+        <v>1</v>
+      </c>
+      <c r="C98" s="2">
+        <v>2</v>
       </c>
       <c r="D98" s="5">
-        <f t="shared" si="27"/>
-        <v>28.4</v>
-      </c>
-      <c r="E98" s="5">
-        <v>0</v>
-      </c>
+        <f t="shared" si="32"/>
+        <v>21.666666666666664</v>
+      </c>
+      <c r="E98" s="5"/>
     </row>
     <row r="99" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="40">
-        <v>4</v>
-      </c>
-      <c r="C99" s="41">
-        <v>1</v>
-      </c>
-      <c r="D99" s="41">
-        <f t="shared" si="27"/>
-        <v>35.599999999999994</v>
-      </c>
-      <c r="E99" s="42"/>
+      <c r="B99" s="2">
+        <v>1</v>
+      </c>
+      <c r="C99" s="2">
+        <v>7</v>
+      </c>
+      <c r="D99" s="40">
+        <f t="shared" si="32"/>
+        <v>60</v>
+      </c>
+      <c r="E99" s="3">
+        <v>60</v>
+      </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="3">
-        <v>1</v>
-      </c>
-      <c r="C100" s="3">
-        <v>6</v>
+      <c r="B100" s="2">
+        <v>5</v>
+      </c>
+      <c r="C100" s="2">
+        <v>1</v>
       </c>
       <c r="D100" s="3">
-        <f t="shared" si="27"/>
-        <v>48</v>
-      </c>
-      <c r="E100" s="3">
-        <v>48</v>
+        <f t="shared" si="32"/>
+        <v>39.333333333333329</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" s="2">
-        <v>7.1999999999999993</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="C101" s="2">
-        <v>6.8000000000000007</v>
+        <v>7.6666666666666661</v>
       </c>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
@@ -4053,21 +4071,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x01010036E71CE10017B64CBC94C9CA9342CDAC" ma:contentTypeVersion="6" ma:contentTypeDescription="Создание документа." ma:contentTypeScope="" ma:versionID="40d9d989aafce748242e11ab5d19c8e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ec24b12e-0b2c-4012-a5eb-d5daf10fd155" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e1a2d6e8a52ec92aaf258989958e158" ns2:_="">
     <xsd:import namespace="ec24b12e-0b2c-4012-a5eb-d5daf10fd155"/>
@@ -4225,31 +4228,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29AC7558-38CF-4C9B-A01D-4F660E7C4C97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B895ACCA-3D6A-43FE-9F30-E99A17535F93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ec24b12e-0b2c-4012-a5eb-d5daf10fd155"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83241ACF-D119-4904-8680-D8081A1C82C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4265,4 +4259,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B895ACCA-3D6A-43FE-9F30-E99A17535F93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ec24b12e-0b2c-4012-a5eb-d5daf10fd155"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29AC7558-38CF-4C9B-A01D-4F660E7C4C97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>